<commit_message>
Skye BDM importers now hopefully complete.
Former-commit-id: dd0318a5d23909ead4724989666978dd5ad6c439
</commit_message>
<xml_diff>
--- a/linkage/src/main/java/uk/ac/standrews/cs/digitising_scotland/linkage/importers/kilmarnock/Skye-Kilmarnock differences.xlsx
+++ b/linkage/src/main/java/uk/ac/standrews/cs/digitising_scotland/linkage/importers/kilmarnock/Skye-Kilmarnock differences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="460" windowWidth="15120" windowHeight="13860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="36120" yWindow="460" windowWidth="15080" windowHeight="26320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Births" sheetId="1" r:id="rId1"/>
@@ -1171,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B37"/>
+    <sheetView topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1396,316 +1396,318 @@
       <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1717,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1756,588 +1758,655 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>98</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>101</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>102</v>
-      </c>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>103</v>
-      </c>
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>107</v>
+      <c r="A25" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>108</v>
+      <c r="A26" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>110</v>
+      <c r="A28" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" t="s">
-        <v>77</v>
+      <c r="A29" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>25</v>
+      <c r="A30" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" t="s">
-        <v>109</v>
+      <c r="A31" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>111</v>
+      <c r="A32" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>112</v>
+      <c r="A33" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>113</v>
+      <c r="A34" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>71</v>
+      <c r="A36" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>72</v>
+      <c r="A37" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>73</v>
+      <c r="A38" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B41" t="s">
-        <v>212</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" t="s">
-        <v>213</v>
+      <c r="A42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" t="s">
-        <v>23</v>
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" t="s">
-        <v>24</v>
+      <c r="A44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" t="s">
-        <v>214</v>
+      <c r="A45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" t="s">
-        <v>74</v>
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" t="s">
-        <v>115</v>
+      <c r="A47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" t="s">
-        <v>215</v>
+      <c r="A48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" t="s">
-        <v>216</v>
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>26</v>
+      <c r="A50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51" t="s">
-        <v>27</v>
+      <c r="A51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" t="s">
-        <v>28</v>
+      <c r="A52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B53" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="A54" s="5"/>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A55" s="5"/>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="A56" s="5"/>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="A57" s="5"/>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" t="s">
-        <v>118</v>
+      <c r="A58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" t="s">
-        <v>119</v>
+      <c r="A59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A60" s="5"/>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="A61" s="5"/>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" t="s">
-        <v>121</v>
+      <c r="A62" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
+      <c r="B64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="5"/>
+      <c r="B68" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="B87" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B64" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+      <c r="B88" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="B89" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B66" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B67" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B68" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B69" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B70" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="B71" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Storr bug (thanks FindBugs for introducing one).
Former-commit-id: a2210dbfe4799efe94b26dadbf19b8b2fc8209c4
</commit_message>
<xml_diff>
--- a/linkage/src/main/java/uk/ac/standrews/cs/digitising_scotland/linkage/importers/kilmarnock/Skye-Kilmarnock differences.xlsx
+++ b/linkage/src/main/java/uk/ac/standrews/cs/digitising_scotland/linkage/importers/kilmarnock/Skye-Kilmarnock differences.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Documents/intelliJ/digitising_scotland/linkage/src/main/java/uk/ac/standrews/cs/digitising_scotland/linkage/importers/kilmarnock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="460" windowWidth="15080" windowHeight="26320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="36120" yWindow="460" windowWidth="15080" windowHeight="26320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Births" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="258">
   <si>
     <t>IOSBIRTH_Identifier</t>
   </si>
@@ -876,8 +876,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -891,11 +893,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1719,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView topLeftCell="A38" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1750,9 +1754,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1854,7 +1856,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1886,526 +1891,521 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>106</v>
+      <c r="A41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>73</v>
+      <c r="A52" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>114</v>
+      <c r="A53" s="5"/>
+      <c r="B53" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" t="s">
-        <v>213</v>
+      <c r="A57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>24</v>
+      <c r="A59" s="5"/>
+      <c r="B59" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" t="s">
-        <v>214</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" t="s">
-        <v>74</v>
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>115</v>
+      <c r="A62" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>116</v>
-      </c>
+      <c r="A63" s="5"/>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" t="s">
-        <v>216</v>
+      <c r="A64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>28</v>
+      <c r="A67" s="5"/>
+      <c r="B67" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="5"/>
-      <c r="B68" t="s">
-        <v>217</v>
+      <c r="A68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>119</v>
+      <c r="A74" s="5"/>
+      <c r="B74" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
-      <c r="B75" t="s">
-        <v>218</v>
+      <c r="A75" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>121</v>
+      <c r="A77" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
-        <v>122</v>
+      <c r="A78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>219</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>46</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>221</v>
+      <c r="B89" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>230</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>231</v>
+      <c r="A101" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2416,13 +2416,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="167" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -2441,635 +2444,707 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>233</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B19" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>235</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>236</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>237</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>238</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>239</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>240</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>241</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>242</v>
-      </c>
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>244</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>245</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>246</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>247</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>145</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>147</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>148</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>150</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>151</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>149</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>152</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>153</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>153</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>156</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>155</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>157</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>158</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>159</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B59" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B60" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B61" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B62" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B63" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B64" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B65" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B67" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B68" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B69" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B70" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B71" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B72" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B73" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B75" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B76" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B77" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B78" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B79" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B80" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" s="5" t="s">
+      <c r="B81" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>160</v>
-      </c>
-      <c r="B62" s="5" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>248</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>249</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>250</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>251</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>252</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>253</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>254</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>255</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>256</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>257</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>